<commit_message>
Update of excel file with V_dis_ye only as trapezoidal form
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Projekte\MA-Model_3\Separator Model\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd1a17303fcb2a19/Documentos/RWTH/Semester 4 (SS25)/MA/W14_Modelle_Auswerten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68857BFD-372D-4503-A341-DFE040420D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4DB114E441178AC67DF4C99614D368683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13F69458-1953-4FC7-9213-3F8969583C4F}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,8 +116,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -127,6 +134,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -394,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,162 +432,162 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
         <v>2.5999999999999998E-4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>160</v>
       </c>
-      <c r="D2">
-        <v>0.2</v>
-      </c>
-      <c r="E2">
+      <c r="D2" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E2" s="1">
         <v>8.7068118117179262E-4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>0.1823660146057291</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
         <v>2.81E-4</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>160</v>
       </c>
-      <c r="D3">
-        <v>0.2</v>
-      </c>
-      <c r="E3">
+      <c r="D3" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="1">
         <v>4.8871695469652121E-4</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>0.21301483549235181</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
         <v>3.0699999999999998E-4</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>160</v>
       </c>
-      <c r="D4">
-        <v>0.2</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E4" s="1">
         <v>5.1845977542828547E-4</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.25425761110318579</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>3.6999999999999999E-4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>160</v>
       </c>
-      <c r="D5">
-        <v>0.2</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="1">
         <v>1.458300691465655E-3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>0.36931815679769697</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
         <v>4.3100000000000001E-4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>160</v>
       </c>
-      <c r="D6">
-        <v>0.2</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="1">
         <v>1.835825293300633E-3</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>0.50113155679252741</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
         <v>5.3200000000000003E-4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>160</v>
       </c>
-      <c r="D7">
-        <v>0.2</v>
-      </c>
-      <c r="E7">
-        <v>1.1514912809325629E-3</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.68696729279858E-3</v>
+      </c>
+      <c r="F7" s="1">
         <v>0.76352010233390366</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
         <v>6.8899999999999994E-4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>160</v>
       </c>
-      <c r="D8">
-        <v>0.2</v>
-      </c>
-      <c r="E8">
-        <v>9.5293032223387007E-4</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.3987886176952151E-3</v>
+      </c>
+      <c r="F8" s="1">
         <v>1.2806653375687329</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
         <v>1.281E-3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>160</v>
       </c>
-      <c r="D9">
-        <v>0.2</v>
-      </c>
-      <c r="E9">
-        <v>7.433338148866344E-4</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.091607149941692E-3</v>
+      </c>
+      <c r="F9" s="1">
         <v>4.4268567706128978</v>
       </c>
     </row>
@@ -694,7 +705,7 @@
         <v>0.2</v>
       </c>
       <c r="E15">
-        <v>1.0761946647764461E-3</v>
+        <v>1.586737251996472E-3</v>
       </c>
       <c r="F15">
         <v>0.73605944943634971</v>
@@ -714,7 +725,7 @@
         <v>0.2</v>
       </c>
       <c r="E16">
-        <v>7.5932554150854605E-4</v>
+        <v>1.1223911989249949E-3</v>
       </c>
       <c r="F16">
         <v>1.3401074860750279</v>
@@ -734,7 +745,7 @@
         <v>0.2</v>
       </c>
       <c r="E17">
-        <v>5.5592191746296098E-4</v>
+        <v>8.2542670588139693E-4</v>
       </c>
       <c r="F17">
         <v>2.5877090019246669</v>
@@ -754,189 +765,189 @@
         <v>0.2</v>
       </c>
       <c r="E18">
-        <v>2.7662656006531691E-4</v>
+        <v>4.1322333877502111E-4</v>
       </c>
       <c r="F18">
         <v>4.8558997971939712</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
         <v>2.7099999999999997E-4</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>240</v>
       </c>
-      <c r="D19">
-        <v>0.2</v>
-      </c>
-      <c r="E19">
+      <c r="D19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="1">
         <v>5.1461472366169756E-4</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="1">
         <v>0.1320822729650824</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
         <v>2.9799999999999998E-4</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>240</v>
       </c>
-      <c r="D20">
-        <v>0.2</v>
-      </c>
-      <c r="E20">
+      <c r="D20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="1">
         <v>1.596125120680681E-3</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="1">
         <v>0.1597123428111161</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
         <v>3.4299999999999999E-4</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>240</v>
       </c>
-      <c r="D21">
-        <v>0.2</v>
-      </c>
-      <c r="E21">
+      <c r="D21" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="1">
         <v>2.5227032600661169E-3</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="1">
         <v>0.211589538977805</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
         <v>4.0400000000000001E-4</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>240</v>
       </c>
-      <c r="D22">
-        <v>0.2</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="1">
         <v>2.8373172099416628E-3</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="1">
         <v>0.29354094122178198</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
         <v>5.0299999999999997E-4</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>240</v>
       </c>
-      <c r="D23">
-        <v>0.2</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="1">
         <v>3.1891748761890149E-3</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.45503198214379609</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1">
         <v>6.0999999999999997E-4</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="1">
         <v>240</v>
       </c>
-      <c r="D24">
-        <v>0.2</v>
-      </c>
-      <c r="E24">
-        <v>1.909077013077547E-3</v>
-      </c>
-      <c r="F24">
+      <c r="D24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="1">
+        <v>2.7472601870201351E-3</v>
+      </c>
+      <c r="F24" s="1">
         <v>0.66921493130958387</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1">
         <v>8.0399999999999992E-4</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="1">
         <v>240</v>
       </c>
-      <c r="D25">
-        <v>0.2</v>
-      </c>
-      <c r="E25">
-        <v>1.451728194097883E-3</v>
-      </c>
-      <c r="F25">
+      <c r="D25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="1">
+        <v>2.0986327494198001E-3</v>
+      </c>
+      <c r="F25" s="1">
         <v>1.162567156778866</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
         <v>1.0920000000000001E-3</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>240</v>
       </c>
-      <c r="D26">
-        <v>0.2</v>
-      </c>
-      <c r="E26">
-        <v>1.158787461713055E-3</v>
-      </c>
-      <c r="F26">
+      <c r="D26" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1.6913322455854431E-3</v>
+      </c>
+      <c r="F26" s="1">
         <v>2.1446243317633749</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27">
+      <c r="A27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1">
         <v>1.4159999999999999E-3</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <v>240</v>
       </c>
-      <c r="D27">
-        <v>0.2</v>
-      </c>
-      <c r="E27">
-        <v>5.9200537170987116E-4</v>
-      </c>
-      <c r="F27">
+      <c r="D27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="1">
+        <v>8.796561944232887E-4</v>
+      </c>
+      <c r="F27" s="1">
         <v>3.606055934726871</v>
       </c>
     </row>
@@ -1074,7 +1085,7 @@
         <v>0.2</v>
       </c>
       <c r="E34">
-        <v>1.877190834877261E-3</v>
+        <v>2.673338910577373E-3</v>
       </c>
       <c r="F34">
         <v>0.98659551435052129</v>
@@ -1094,7 +1105,7 @@
         <v>0.2</v>
       </c>
       <c r="E35">
-        <v>1.5326450942369911E-3</v>
+        <v>2.1898914426851492E-3</v>
       </c>
       <c r="F35">
         <v>1.8618922637938651</v>
@@ -1114,289 +1125,289 @@
         <v>0.2</v>
       </c>
       <c r="E36">
-        <v>9.4351313076291188E-4</v>
+        <v>1.3911121113393721E-3</v>
       </c>
       <c r="F36">
         <v>2.5177979188444941</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>6.9999999999999999E-4</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="1">
         <v>2050</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>0.3</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>9.0499999999999999E-4</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="1">
         <v>2350</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>0.5</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>6.3250000000000003E-4</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="1">
         <v>1600</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>0.3</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>6.0749999999999997E-4</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="1">
         <v>1500</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>0.3</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>7.3800000000000005E-4</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="1">
         <v>1450</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>0.5</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>8.6499999999999999E-4</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="1">
         <v>1850</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>0.5</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>6.2750000000000002E-4</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="1">
         <v>1600</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>0.3</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>5.8500000000000002E-4</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="1">
         <v>1450</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>0.3</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>7.0750000000000001E-4</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="1">
         <v>1400</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>0.5</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>6.3500000000000004E-4</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="1">
         <v>1150</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>0.5</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>6.6750000000000002E-4</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="1">
         <v>1600</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>0.3</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>6.3029999999999998E-4</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="1">
         <v>1500</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>0.3</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>7.2250000000000005E-4</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="1">
         <v>1350</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>0.5</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>6.7250000000000003E-4</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="1">
         <v>1200</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>0.5</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="1">
         <v>5.9087441444048081E-3</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Re-Calculation of V_dis_ye to 2L_DPZ/3
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd1a17303fcb2a19/Documentos/RWTH/Semester 4 (SS25)/MA/W14_Modelle_Auswerten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4DB114E441178AC67DF4C99614D368683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13F69458-1953-4FC7-9213-3F8969583C4F}"/>
+  <xr:revisionPtr revIDLastSave="103" documentId="11_AD4DB114E441178AC67DF4C99614D368683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{069B8A25-7133-496C-9455-6B0B2823A8F0}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +445,7 @@
         <v>0.2</v>
       </c>
       <c r="E2" s="1">
-        <v>8.7068118117179262E-4</v>
+        <v>9.6295716614565059E-4</v>
       </c>
       <c r="F2" s="1">
         <v>0.1823660146057291</v>
@@ -465,7 +465,7 @@
         <v>0.2</v>
       </c>
       <c r="E3" s="1">
-        <v>4.8871695469652121E-4</v>
+        <v>5.4068508635758987E-4</v>
       </c>
       <c r="F3" s="1">
         <v>0.21301483549235181</v>
@@ -485,7 +485,7 @@
         <v>0.2</v>
       </c>
       <c r="E4" s="1">
-        <v>5.1845977542828547E-4</v>
+        <v>5.7356177557115905E-4</v>
       </c>
       <c r="F4" s="1">
         <v>0.25425761110318579</v>
@@ -505,7 +505,7 @@
         <v>0.2</v>
       </c>
       <c r="E5" s="1">
-        <v>1.458300691465655E-3</v>
+        <v>1.6091137159752529E-3</v>
       </c>
       <c r="F5" s="1">
         <v>0.36931815679769697</v>
@@ -525,7 +525,7 @@
         <v>0.2</v>
       </c>
       <c r="E6" s="1">
-        <v>1.835825293300633E-3</v>
+        <v>2.022104184845368E-3</v>
       </c>
       <c r="F6" s="1">
         <v>0.50113155679252741</v>
@@ -545,7 +545,7 @@
         <v>0.2</v>
       </c>
       <c r="E7" s="1">
-        <v>1.68696729279858E-3</v>
+        <v>1.8583168791360669E-3</v>
       </c>
       <c r="F7" s="1">
         <v>0.76352010233390366</v>
@@ -565,7 +565,7 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="1">
-        <v>1.3987886176952151E-3</v>
+        <v>1.5414611966421831E-3</v>
       </c>
       <c r="F8" s="1">
         <v>1.2806653375687329</v>
@@ -585,7 +585,7 @@
         <v>0.2</v>
       </c>
       <c r="E9" s="1">
-        <v>1.091607149941692E-3</v>
+        <v>1.203053031576804E-3</v>
       </c>
       <c r="F9" s="1">
         <v>4.4268567706128978</v>
@@ -605,7 +605,7 @@
         <v>0.2</v>
       </c>
       <c r="E10">
-        <v>2.0578457107418729E-4</v>
+        <v>2.2772938978669619E-4</v>
       </c>
       <c r="F10">
         <v>0.1370529158760026</v>
@@ -625,7 +625,7 @@
         <v>0.2</v>
       </c>
       <c r="E11">
-        <v>1.218968850821466E-3</v>
+        <v>1.3477410867637691E-3</v>
       </c>
       <c r="F11">
         <v>0.17284629282554129</v>
@@ -645,7 +645,7 @@
         <v>0.2</v>
       </c>
       <c r="E12">
-        <v>1.3407609059908621E-3</v>
+        <v>1.48167952704679E-3</v>
       </c>
       <c r="F12">
         <v>0.2279575182571614</v>
@@ -665,7 +665,7 @@
         <v>0.2</v>
       </c>
       <c r="E13">
-        <v>1.4324225232782979E-3</v>
+        <v>1.5823525896206921E-3</v>
       </c>
       <c r="F13">
         <v>0.31658092682248279</v>
@@ -685,7 +685,7 @@
         <v>0.2</v>
       </c>
       <c r="E14">
-        <v>1.1444992140372311E-3</v>
+        <v>1.2640770242587729E-3</v>
       </c>
       <c r="F14">
         <v>0.46464702343852138</v>
@@ -705,7 +705,7 @@
         <v>0.2</v>
       </c>
       <c r="E15">
-        <v>1.586737251996472E-3</v>
+        <v>1.750109021017441E-3</v>
       </c>
       <c r="F15">
         <v>0.73605944943634971</v>
@@ -725,7 +725,7 @@
         <v>0.2</v>
       </c>
       <c r="E16">
-        <v>1.1223911989249949E-3</v>
+        <v>1.238571092807607E-3</v>
       </c>
       <c r="F16">
         <v>1.3401074860750279</v>
@@ -745,7 +745,7 @@
         <v>0.2</v>
       </c>
       <c r="E17">
-        <v>8.2542670588139693E-4</v>
+        <v>9.1166767204117576E-4</v>
       </c>
       <c r="F17">
         <v>2.5877090019246669</v>
@@ -765,7 +765,7 @@
         <v>0.2</v>
       </c>
       <c r="E18">
-        <v>4.1322333877502111E-4</v>
+        <v>4.5693419373077951E-4</v>
       </c>
       <c r="F18">
         <v>4.8558997971939712</v>
@@ -785,7 +785,7 @@
         <v>0.2</v>
       </c>
       <c r="E19" s="1">
-        <v>5.1461472366169756E-4</v>
+        <v>5.6943586866757242E-4</v>
       </c>
       <c r="F19" s="1">
         <v>0.1320822729650824</v>
@@ -805,7 +805,7 @@
         <v>0.2</v>
       </c>
       <c r="E20" s="1">
-        <v>1.596125120680681E-3</v>
+        <v>1.7641118244044319E-3</v>
       </c>
       <c r="F20" s="1">
         <v>0.1597123428111161</v>
@@ -825,7 +825,7 @@
         <v>0.2</v>
       </c>
       <c r="E21" s="1">
-        <v>2.5227032600661169E-3</v>
+        <v>2.7815827299968472E-3</v>
       </c>
       <c r="F21" s="1">
         <v>0.211589538977805</v>
@@ -845,7 +845,7 @@
         <v>0.2</v>
       </c>
       <c r="E22" s="1">
-        <v>2.8373172099416628E-3</v>
+        <v>3.1243836337864731E-3</v>
       </c>
       <c r="F22" s="1">
         <v>0.29354094122178198</v>
@@ -865,7 +865,7 @@
         <v>0.2</v>
       </c>
       <c r="E23" s="1">
-        <v>3.1891748761890149E-3</v>
+        <v>3.5047858321507158E-3</v>
       </c>
       <c r="F23" s="1">
         <v>0.45503198214379609</v>
@@ -885,7 +885,7 @@
         <v>0.2</v>
       </c>
       <c r="E24" s="1">
-        <v>2.7472601870201351E-3</v>
+        <v>3.0154706835275259E-3</v>
       </c>
       <c r="F24" s="1">
         <v>0.66921493130958387</v>
@@ -905,7 +905,7 @@
         <v>0.2</v>
       </c>
       <c r="E25" s="1">
-        <v>2.0986327494198001E-3</v>
+        <v>2.3056367382307788E-3</v>
       </c>
       <c r="F25" s="1">
         <v>1.162567156778866</v>
@@ -925,7 +925,7 @@
         <v>0.2</v>
       </c>
       <c r="E26" s="1">
-        <v>1.6913322455854431E-3</v>
+        <v>1.8617433763087039E-3</v>
       </c>
       <c r="F26" s="1">
         <v>2.1446243317633749</v>
@@ -945,7 +945,7 @@
         <v>0.2</v>
       </c>
       <c r="E27" s="1">
-        <v>8.796561944232887E-4</v>
+        <v>9.7170389896743172E-4</v>
       </c>
       <c r="F27" s="1">
         <v>3.606055934726871</v>
@@ -985,7 +985,7 @@
         <v>0.2</v>
       </c>
       <c r="E29">
-        <v>2.248917137399704E-3</v>
+        <v>2.481912581033939E-3</v>
       </c>
       <c r="F29">
         <v>0.13324589043500251</v>
@@ -1005,7 +1005,7 @@
         <v>0.2</v>
       </c>
       <c r="E30">
-        <v>3.1891748761890149E-3</v>
+        <v>3.5047858321507158E-3</v>
       </c>
       <c r="F30">
         <v>0.17507291557699109</v>
@@ -1025,7 +1025,7 @@
         <v>0.2</v>
       </c>
       <c r="E31">
-        <v>3.2126682172198069E-3</v>
+        <v>3.5300274842651859E-3</v>
       </c>
       <c r="F31">
         <v>0.24912153359547129</v>
@@ -1045,7 +1045,7 @@
         <v>0.2</v>
       </c>
       <c r="E32">
-        <v>3.4195819994518669E-3</v>
+        <v>3.7511155850126609E-3</v>
       </c>
       <c r="F32">
         <v>0.38077808031907501</v>
@@ -1065,7 +1065,7 @@
         <v>0.2</v>
       </c>
       <c r="E33">
-        <v>3.4579550590871861E-3</v>
+        <v>3.7918205784826329E-3</v>
       </c>
       <c r="F33">
         <v>0.58685321837904003</v>
@@ -1085,7 +1085,7 @@
         <v>0.2</v>
       </c>
       <c r="E34">
-        <v>2.673338910577373E-3</v>
+        <v>2.9280961559260119E-3</v>
       </c>
       <c r="F34">
         <v>0.98659551435052129</v>
@@ -1105,7 +1105,7 @@
         <v>0.2</v>
       </c>
       <c r="E35">
-        <v>2.1898914426851492E-3</v>
+        <v>2.4002025628507462E-3</v>
       </c>
       <c r="F35">
         <v>1.8618922637938651</v>
@@ -1125,7 +1125,7 @@
         <v>0.2</v>
       </c>
       <c r="E36">
-        <v>1.3911121113393721E-3</v>
+        <v>1.53434215541255E-3</v>
       </c>
       <c r="F36">
         <v>2.5177979188444941</v>

</xml_diff>

<commit_message>
Added all detail test to data_main.xlsx. Also updated parallel code for running detail tests. Ready to run.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagr9\Projekte\MA\MA-Model_3\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40ED897-035D-4198-A3BF-97B569D9722E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4B3506-46E1-4AF3-A88C-9FD61A206621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4620" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="sozh" sheetId="2" r:id="rId2"/>
+    <sheet name="detail_V_dis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="21">
   <si>
     <t>exp</t>
   </si>
@@ -106,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +129,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -143,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,15 +160,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2405,7 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11386E68-8A5F-41CC-B5E5-AE3FA3B0350A}">
   <dimension ref="A1:H363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+    <sheetView topLeftCell="A327" workbookViewId="0">
       <selection activeCell="G363" sqref="G363"/>
     </sheetView>
   </sheetViews>
@@ -11852,4 +11877,2749 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20356976-3232-4BA6-902F-5E9FBCFC61E6}">
+  <dimension ref="A1:H105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>2.0462099999999999E-4</v>
+      </c>
+      <c r="C2">
+        <v>743.10170100000005</v>
+      </c>
+      <c r="D2">
+        <v>0.29701893400000001</v>
+      </c>
+      <c r="E2">
+        <v>3.6502927999999997E-2</v>
+      </c>
+      <c r="F2">
+        <v>9.6633421999999997E-2</v>
+      </c>
+      <c r="G2">
+        <v>4.4652340000000002E-3</v>
+      </c>
+      <c r="H2">
+        <v>0.98750888400000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>6.5725699999999996E-4</v>
+      </c>
+      <c r="C3">
+        <v>748.36788460000002</v>
+      </c>
+      <c r="D3">
+        <v>0.50333939500000002</v>
+      </c>
+      <c r="E3">
+        <v>2.8484735000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.2660582000000005E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.528742E-3</v>
+      </c>
+      <c r="H3">
+        <v>0.99108918400000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>3.1127999999999999E-4</v>
+      </c>
+      <c r="C4">
+        <v>749.92972780000002</v>
+      </c>
+      <c r="D4">
+        <v>0.49988101000000001</v>
+      </c>
+      <c r="E4">
+        <v>3.8919571E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.10772396300000001</v>
+      </c>
+      <c r="G4">
+        <v>4.7552549999999999E-3</v>
+      </c>
+      <c r="H4">
+        <v>0.99268671900000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>4.4927699999999999E-4</v>
+      </c>
+      <c r="C5">
+        <v>749.97402599999998</v>
+      </c>
+      <c r="D5">
+        <v>0.399764919</v>
+      </c>
+      <c r="E5">
+        <v>3.8463404E-2</v>
+      </c>
+      <c r="F5">
+        <v>9.5001253999999993E-2</v>
+      </c>
+      <c r="G5">
+        <v>3.785549E-3</v>
+      </c>
+      <c r="H5">
+        <v>0.98653263199999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>5.4967899999999997E-4</v>
+      </c>
+      <c r="C6">
+        <v>750.02556879999997</v>
+      </c>
+      <c r="D6">
+        <v>0.50015754999999995</v>
+      </c>
+      <c r="E6">
+        <v>4.0361706999999997E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.101830843</v>
+      </c>
+      <c r="G6">
+        <v>5.2321299999999998E-3</v>
+      </c>
+      <c r="H6">
+        <v>0.99445781600000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>3.38769E-4</v>
+      </c>
+      <c r="C7">
+        <v>750.05733190000001</v>
+      </c>
+      <c r="D7">
+        <v>0.49989457599999998</v>
+      </c>
+      <c r="E7">
+        <v>3.8023349999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.108397884</v>
+      </c>
+      <c r="G7">
+        <v>4.1389720000000003E-3</v>
+      </c>
+      <c r="H7">
+        <v>0.99176721899999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2.4194099999999999E-4</v>
+      </c>
+      <c r="C8">
+        <v>750.20782199999996</v>
+      </c>
+      <c r="D8">
+        <v>0.40002338700000001</v>
+      </c>
+      <c r="E8">
+        <v>6.6916982E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.106790285</v>
+      </c>
+      <c r="G8">
+        <v>5.2340670000000002E-3</v>
+      </c>
+      <c r="H8">
+        <v>0.99171526700000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>4.9274500000000005E-4</v>
+      </c>
+      <c r="C9">
+        <v>750.25178530000005</v>
+      </c>
+      <c r="D9">
+        <v>0.29988877800000002</v>
+      </c>
+      <c r="E9">
+        <v>3.6448479999999998E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.10019613600000001</v>
+      </c>
+      <c r="G9">
+        <v>2.8000159999999998E-3</v>
+      </c>
+      <c r="H9">
+        <v>0.98938694400000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>6.1183099999999996E-4</v>
+      </c>
+      <c r="C10">
+        <v>750.71744000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.50033280999999996</v>
+      </c>
+      <c r="E10">
+        <v>3.7521118999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>9.8495864000000002E-2</v>
+      </c>
+      <c r="G10">
+        <v>3.1483090000000002E-3</v>
+      </c>
+      <c r="H10">
+        <v>0.99218971899999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>3.9097999999999997E-4</v>
+      </c>
+      <c r="C11">
+        <v>750.86723619999998</v>
+      </c>
+      <c r="D11">
+        <v>0.30092750000000001</v>
+      </c>
+      <c r="E11">
+        <v>3.3229887E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.100884113</v>
+      </c>
+      <c r="G11">
+        <v>3.2887580000000001E-3</v>
+      </c>
+      <c r="H11">
+        <v>0.99199386300000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2.2167000000000001E-4</v>
+      </c>
+      <c r="C12">
+        <v>751.48936860000003</v>
+      </c>
+      <c r="D12">
+        <v>0.40003253100000002</v>
+      </c>
+      <c r="E12">
+        <v>7.0955006000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.11041532699999999</v>
+      </c>
+      <c r="G12">
+        <v>4.5576050000000002E-3</v>
+      </c>
+      <c r="H12">
+        <v>0.99505433700000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>6.7796600000000001E-4</v>
+      </c>
+      <c r="C13">
+        <v>752.85933369999998</v>
+      </c>
+      <c r="D13">
+        <v>0.49949943499999999</v>
+      </c>
+      <c r="E13">
+        <v>4.2382797999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.7580385000000006E-2</v>
+      </c>
+      <c r="G13">
+        <v>3.6210349999999999E-3</v>
+      </c>
+      <c r="H13">
+        <v>0.99436792399999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>2.54348E-4</v>
+      </c>
+      <c r="C14">
+        <v>908.35374130000002</v>
+      </c>
+      <c r="D14">
+        <v>0.27718706700000001</v>
+      </c>
+      <c r="E14">
+        <v>3.6368708E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.103970942</v>
+      </c>
+      <c r="G14">
+        <v>3.6805710000000001E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.99263151500000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>8.0239500000000002E-4</v>
+      </c>
+      <c r="C15">
+        <v>998.44373169999994</v>
+      </c>
+      <c r="D15">
+        <v>0.499859416</v>
+      </c>
+      <c r="E15">
+        <v>1.8851822000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.10280117799999999</v>
+      </c>
+      <c r="G15">
+        <v>3.8602500000000002E-4</v>
+      </c>
+      <c r="H15">
+        <v>0.99546705300000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>5.0275999999999999E-4</v>
+      </c>
+      <c r="C16">
+        <v>999.40820970000004</v>
+      </c>
+      <c r="D16">
+        <v>0.29920427599999999</v>
+      </c>
+      <c r="E16">
+        <v>4.1816536000000001E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.101860464</v>
+      </c>
+      <c r="G16">
+        <v>4.1493759999999998E-3</v>
+      </c>
+      <c r="H16">
+        <v>0.98989876499999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>5.9944000000000002E-4</v>
+      </c>
+      <c r="C17">
+        <v>999.59662909999997</v>
+      </c>
+      <c r="D17">
+        <v>0.40006547100000001</v>
+      </c>
+      <c r="E17">
+        <v>2.4784075999999999E-2</v>
+      </c>
+      <c r="F17">
+        <v>9.7689174000000004E-2</v>
+      </c>
+      <c r="G17">
+        <v>4.8635799999999999E-4</v>
+      </c>
+      <c r="H17">
+        <v>0.99499302099999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>7.1244500000000003E-4</v>
+      </c>
+      <c r="C18">
+        <v>999.64467930000001</v>
+      </c>
+      <c r="D18">
+        <v>0.49991358299999999</v>
+      </c>
+      <c r="E18">
+        <v>1.8550810000000001E-2</v>
+      </c>
+      <c r="F18">
+        <v>9.4884389999999999E-2</v>
+      </c>
+      <c r="G18">
+        <v>2.2179650000000001E-3</v>
+      </c>
+      <c r="H18">
+        <v>0.99704778699999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>3.7785800000000001E-4</v>
+      </c>
+      <c r="C19">
+        <v>999.67359969999995</v>
+      </c>
+      <c r="D19">
+        <v>0.30006925000000001</v>
+      </c>
+      <c r="E19">
+        <v>3.6809690999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.108183192</v>
+      </c>
+      <c r="G19">
+        <v>4.052745E-3</v>
+      </c>
+      <c r="H19">
+        <v>0.98579144299999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>5.6844399999999998E-4</v>
+      </c>
+      <c r="C20">
+        <v>1000.032227</v>
+      </c>
+      <c r="D20">
+        <v>0.29996158899999997</v>
+      </c>
+      <c r="E20">
+        <v>1.9367124999999999E-2</v>
+      </c>
+      <c r="F20">
+        <v>9.7314092000000005E-2</v>
+      </c>
+      <c r="G20">
+        <v>2.175696E-3</v>
+      </c>
+      <c r="H20">
+        <v>0.995888047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>6.5962200000000001E-4</v>
+      </c>
+      <c r="C21">
+        <v>1000.129858</v>
+      </c>
+      <c r="D21">
+        <v>0.49965211700000001</v>
+      </c>
+      <c r="E21">
+        <v>4.2670694000000002E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.10375522299999999</v>
+      </c>
+      <c r="G21">
+        <v>5.4323920000000003E-3</v>
+      </c>
+      <c r="H21">
+        <v>0.99410157700000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>7.5361500000000001E-4</v>
+      </c>
+      <c r="C22">
+        <v>1000.183129</v>
+      </c>
+      <c r="D22">
+        <v>0.50001522700000001</v>
+      </c>
+      <c r="E22">
+        <v>1.9893559000000002E-2</v>
+      </c>
+      <c r="F22">
+        <v>9.5239508E-2</v>
+      </c>
+      <c r="G22">
+        <v>2.0156449999999999E-3</v>
+      </c>
+      <c r="H22">
+        <v>0.99718886500000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>3.65507E-4</v>
+      </c>
+      <c r="C23">
+        <v>1000.201091</v>
+      </c>
+      <c r="D23">
+        <v>0.30000356700000003</v>
+      </c>
+      <c r="E23">
+        <v>5.1118615999999999E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.114449734</v>
+      </c>
+      <c r="G23">
+        <v>4.440495E-3</v>
+      </c>
+      <c r="H23">
+        <v>0.99139601200000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>3.21902E-4</v>
+      </c>
+      <c r="C24">
+        <v>1000.303949</v>
+      </c>
+      <c r="D24">
+        <v>0.50013415000000006</v>
+      </c>
+      <c r="E24">
+        <v>5.7089112999999997E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.11521322000000001</v>
+      </c>
+      <c r="G24">
+        <v>4.8777610000000004E-3</v>
+      </c>
+      <c r="H24">
+        <v>0.99550441999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>4.4690600000000001E-4</v>
+      </c>
+      <c r="C25">
+        <v>1000.564352</v>
+      </c>
+      <c r="D25">
+        <v>0.40118413600000002</v>
+      </c>
+      <c r="E25">
+        <v>4.5435773999999998E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.10055367599999999</v>
+      </c>
+      <c r="G25">
+        <v>4.5400780000000003E-3</v>
+      </c>
+      <c r="H25">
+        <v>0.98875126400000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>2.6539199999999998E-4</v>
+      </c>
+      <c r="C26">
+        <v>1002.961609</v>
+      </c>
+      <c r="D26">
+        <v>0.30087852900000001</v>
+      </c>
+      <c r="E26">
+        <v>7.5760642000000003E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.10911349100000001</v>
+      </c>
+      <c r="G26">
+        <v>5.1225200000000002E-3</v>
+      </c>
+      <c r="H26">
+        <v>0.99228384400000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>2.7240599999999999E-4</v>
+      </c>
+      <c r="C27">
+        <v>1242.8563799999999</v>
+      </c>
+      <c r="D27">
+        <v>0.29883443599999998</v>
+      </c>
+      <c r="E27">
+        <v>6.6170259999999995E-2</v>
+      </c>
+      <c r="F27">
+        <v>0.11349644</v>
+      </c>
+      <c r="G27">
+        <v>5.5628220000000003E-3</v>
+      </c>
+      <c r="H27">
+        <v>0.99175836900000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>5.6636299999999996E-4</v>
+      </c>
+      <c r="C28">
+        <v>1249.038305</v>
+      </c>
+      <c r="D28">
+        <v>0.50009379399999998</v>
+      </c>
+      <c r="E28">
+        <v>5.5513298000000003E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.114298685</v>
+      </c>
+      <c r="G28">
+        <v>5.8367810000000001E-3</v>
+      </c>
+      <c r="H28">
+        <v>0.99043759600000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>4.4455299999999998E-4</v>
+      </c>
+      <c r="C29">
+        <v>1249.8621929999999</v>
+      </c>
+      <c r="D29">
+        <v>0.29980042600000001</v>
+      </c>
+      <c r="E29">
+        <v>3.1885854999999998E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.10856081200000001</v>
+      </c>
+      <c r="G29">
+        <v>3.8722560000000001E-3</v>
+      </c>
+      <c r="H29">
+        <v>0.98956896599999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>3.4781999999999999E-4</v>
+      </c>
+      <c r="C30">
+        <v>1249.9720520000001</v>
+      </c>
+      <c r="D30">
+        <v>0.29999618500000003</v>
+      </c>
+      <c r="E30">
+        <v>4.7035642000000003E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.10975439100000001</v>
+      </c>
+      <c r="G30">
+        <v>4.7517119999999999E-3</v>
+      </c>
+      <c r="H30">
+        <v>0.98241363800000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31">
+        <v>3.0862499999999998E-4</v>
+      </c>
+      <c r="C31">
+        <v>1250.009063</v>
+      </c>
+      <c r="D31">
+        <v>0.300016848</v>
+      </c>
+      <c r="E31">
+        <v>4.267257E-2</v>
+      </c>
+      <c r="F31">
+        <v>0.107568497</v>
+      </c>
+      <c r="G31">
+        <v>4.6496790000000003E-3</v>
+      </c>
+      <c r="H31">
+        <v>0.98361751799999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <v>3.9580799999999999E-4</v>
+      </c>
+      <c r="C32">
+        <v>1250.0364039999999</v>
+      </c>
+      <c r="D32">
+        <v>0.29999587</v>
+      </c>
+      <c r="E32">
+        <v>4.6113999000000003E-2</v>
+      </c>
+      <c r="F32">
+        <v>0.11548971800000001</v>
+      </c>
+      <c r="G32">
+        <v>4.2850120000000004E-3</v>
+      </c>
+      <c r="H32">
+        <v>0.99005631800000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4.85129E-4</v>
+      </c>
+      <c r="C33">
+        <v>1250.056002</v>
+      </c>
+      <c r="D33">
+        <v>0.30007985999999998</v>
+      </c>
+      <c r="E33">
+        <v>3.1432143000000003E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.11381099</v>
+      </c>
+      <c r="G33">
+        <v>4.0394979999999999E-3</v>
+      </c>
+      <c r="H33">
+        <v>0.99273382399999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>4.7428800000000001E-4</v>
+      </c>
+      <c r="C34">
+        <v>1250.0886849999999</v>
+      </c>
+      <c r="D34">
+        <v>0.30001281800000001</v>
+      </c>
+      <c r="E34">
+        <v>3.3010744000000002E-2</v>
+      </c>
+      <c r="F34">
+        <v>0.11308117199999999</v>
+      </c>
+      <c r="G34">
+        <v>5.2047889999999996E-3</v>
+      </c>
+      <c r="H34">
+        <v>0.99108814999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>3.4672300000000001E-4</v>
+      </c>
+      <c r="C35">
+        <v>1250.9434040000001</v>
+      </c>
+      <c r="D35">
+        <v>0.39999618199999998</v>
+      </c>
+      <c r="E35">
+        <v>6.9506928999999995E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.110695898</v>
+      </c>
+      <c r="G35">
+        <v>6.4767380000000001E-3</v>
+      </c>
+      <c r="H35">
+        <v>0.99251876100000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>5.7827599999999996E-4</v>
+      </c>
+      <c r="C36">
+        <v>1252.670832</v>
+      </c>
+      <c r="D36">
+        <v>0.49995556099999999</v>
+      </c>
+      <c r="E36">
+        <v>4.8558603999999998E-2</v>
+      </c>
+      <c r="F36">
+        <v>9.5985962999999994E-2</v>
+      </c>
+      <c r="G36">
+        <v>5.6972220000000001E-3</v>
+      </c>
+      <c r="H36">
+        <v>0.98525604600000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>4.6433100000000001E-4</v>
+      </c>
+      <c r="C37">
+        <v>1255.424561</v>
+      </c>
+      <c r="D37">
+        <v>0.39989443400000002</v>
+      </c>
+      <c r="E37">
+        <v>4.1705930000000002E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.10475915299999999</v>
+      </c>
+      <c r="G37">
+        <v>4.4100290000000002E-3</v>
+      </c>
+      <c r="H37">
+        <v>0.98489914300000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>4.11395E-4</v>
+      </c>
+      <c r="C38">
+        <v>1267.5140690000001</v>
+      </c>
+      <c r="D38">
+        <v>0.49920661399999999</v>
+      </c>
+      <c r="E38">
+        <v>4.8344787E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.12562072899999999</v>
+      </c>
+      <c r="G38">
+        <v>3.9256580000000003E-3</v>
+      </c>
+      <c r="H38">
+        <v>0.99312282299999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>3.13467E-4</v>
+      </c>
+      <c r="C39">
+        <v>1271.3936630000001</v>
+      </c>
+      <c r="D39">
+        <v>0.40056073800000003</v>
+      </c>
+      <c r="E39">
+        <v>7.1139833E-2</v>
+      </c>
+      <c r="F39">
+        <v>0.11312243299999999</v>
+      </c>
+      <c r="G39">
+        <v>5.9295399999999996E-3</v>
+      </c>
+      <c r="H39">
+        <v>0.99374623100000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>7.2654800000000004E-4</v>
+      </c>
+      <c r="C40">
+        <v>1455.6305829999999</v>
+      </c>
+      <c r="D40">
+        <v>0.49692148400000002</v>
+      </c>
+      <c r="E40">
+        <v>2.3973168999999999E-2</v>
+      </c>
+      <c r="F40">
+        <v>9.1711663999999998E-2</v>
+      </c>
+      <c r="G40">
+        <v>2.966729E-3</v>
+      </c>
+      <c r="H40">
+        <v>0.99718670099999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>8.1662800000000002E-4</v>
+      </c>
+      <c r="C41">
+        <v>1492.737848</v>
+      </c>
+      <c r="D41">
+        <v>0.50025813699999999</v>
+      </c>
+      <c r="E41">
+        <v>2.6577284999999999E-2</v>
+      </c>
+      <c r="F41">
+        <v>9.2475197999999995E-2</v>
+      </c>
+      <c r="G41">
+        <v>2.9827109999999999E-3</v>
+      </c>
+      <c r="H41">
+        <v>0.99533773199999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>8.5975099999999996E-4</v>
+      </c>
+      <c r="C42">
+        <v>1494.673636</v>
+      </c>
+      <c r="D42">
+        <v>0.50000099099999995</v>
+      </c>
+      <c r="E42">
+        <v>2.6915963000000001E-2</v>
+      </c>
+      <c r="F42">
+        <v>9.1934420000000003E-2</v>
+      </c>
+      <c r="G42">
+        <v>2.846627E-3</v>
+      </c>
+      <c r="H42">
+        <v>0.99697522500000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>7.0617800000000001E-4</v>
+      </c>
+      <c r="C43">
+        <v>1497.1705119999999</v>
+      </c>
+      <c r="D43">
+        <v>0.49990232400000001</v>
+      </c>
+      <c r="E43">
+        <v>2.4668497000000001E-2</v>
+      </c>
+      <c r="F43">
+        <v>9.1588153000000005E-2</v>
+      </c>
+      <c r="G43">
+        <v>3.0430520000000001E-3</v>
+      </c>
+      <c r="H43">
+        <v>0.99707969600000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>6.3737199999999998E-4</v>
+      </c>
+      <c r="C44">
+        <v>1500.051467</v>
+      </c>
+      <c r="D44">
+        <v>0.29994249899999997</v>
+      </c>
+      <c r="E44">
+        <v>2.6047677000000002E-2</v>
+      </c>
+      <c r="F44">
+        <v>0.10857765</v>
+      </c>
+      <c r="G44">
+        <v>7.1048200000000002E-4</v>
+      </c>
+      <c r="H44">
+        <v>0.99349073799999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>5.2616900000000005E-4</v>
+      </c>
+      <c r="C45">
+        <v>1500.0874120000001</v>
+      </c>
+      <c r="D45">
+        <v>0.30007125099999998</v>
+      </c>
+      <c r="E45">
+        <v>1.9110674000000001E-2</v>
+      </c>
+      <c r="F45">
+        <v>0.12915310899999999</v>
+      </c>
+      <c r="G45">
+        <v>7.8471699999999999E-4</v>
+      </c>
+      <c r="H45">
+        <v>0.99525415699999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>7.4180700000000003E-4</v>
+      </c>
+      <c r="C46">
+        <v>1500.215265</v>
+      </c>
+      <c r="D46">
+        <v>0.39993976599999997</v>
+      </c>
+      <c r="E46">
+        <v>2.7369943000000001E-2</v>
+      </c>
+      <c r="F46">
+        <v>9.7766817000000006E-2</v>
+      </c>
+      <c r="G46">
+        <v>4.3964299999999998E-4</v>
+      </c>
+      <c r="H46">
+        <v>0.99480906899999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47">
+        <v>9.1292700000000001E-4</v>
+      </c>
+      <c r="C47">
+        <v>1500.5413000000001</v>
+      </c>
+      <c r="D47">
+        <v>0.50044513199999996</v>
+      </c>
+      <c r="E47">
+        <v>2.0620128000000001E-2</v>
+      </c>
+      <c r="F47">
+        <v>0.103834646</v>
+      </c>
+      <c r="G47">
+        <v>4.4096199999999998E-4</v>
+      </c>
+      <c r="H47">
+        <v>0.99445706499999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <v>9.4360899999999998E-4</v>
+      </c>
+      <c r="C48">
+        <v>1500.993866</v>
+      </c>
+      <c r="D48">
+        <v>0.499986655</v>
+      </c>
+      <c r="E48">
+        <v>2.1720821000000001E-2</v>
+      </c>
+      <c r="F48">
+        <v>0.103615651</v>
+      </c>
+      <c r="G48">
+        <v>8.3131500000000001E-4</v>
+      </c>
+      <c r="H48">
+        <v>0.99464200000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>6.1466400000000001E-4</v>
+      </c>
+      <c r="C49">
+        <v>1502.4972680000001</v>
+      </c>
+      <c r="D49">
+        <v>0.40017336999999997</v>
+      </c>
+      <c r="E49">
+        <v>2.0735538000000001E-2</v>
+      </c>
+      <c r="F49">
+        <v>9.4777095000000006E-2</v>
+      </c>
+      <c r="G49">
+        <v>2.47956E-3</v>
+      </c>
+      <c r="H49">
+        <v>0.99691817900000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>6.6162899999999995E-4</v>
+      </c>
+      <c r="C50">
+        <v>1504.5464079999999</v>
+      </c>
+      <c r="D50">
+        <v>0.40074769799999999</v>
+      </c>
+      <c r="E50">
+        <v>2.2464746000000001E-2</v>
+      </c>
+      <c r="F50">
+        <v>9.4852504000000004E-2</v>
+      </c>
+      <c r="G50">
+        <v>2.9607710000000001E-3</v>
+      </c>
+      <c r="H50">
+        <v>0.99641502000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>7.2370699999999997E-4</v>
+      </c>
+      <c r="C51">
+        <v>1752.5926159999999</v>
+      </c>
+      <c r="D51">
+        <v>0.50002069100000002</v>
+      </c>
+      <c r="E51">
+        <v>2.4334100000000001E-2</v>
+      </c>
+      <c r="F51">
+        <v>9.0262732999999998E-2</v>
+      </c>
+      <c r="G51">
+        <v>2.7651020000000002E-3</v>
+      </c>
+      <c r="H51">
+        <v>0.99688110399999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52">
+        <v>8.0128199999999995E-4</v>
+      </c>
+      <c r="C52">
+        <v>1995.9935250000001</v>
+      </c>
+      <c r="D52">
+        <v>0.49970003499999999</v>
+      </c>
+      <c r="E52">
+        <v>2.3888031000000001E-2</v>
+      </c>
+      <c r="F52">
+        <v>0.101849986</v>
+      </c>
+      <c r="G52">
+        <v>6.1271999999999997E-4</v>
+      </c>
+      <c r="H52">
+        <v>0.99330616800000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>6.8117199999999996E-4</v>
+      </c>
+      <c r="C53">
+        <v>1999.6194820000001</v>
+      </c>
+      <c r="D53">
+        <v>0.49998881699999997</v>
+      </c>
+      <c r="E53">
+        <v>2.6883537999999998E-2</v>
+      </c>
+      <c r="F53">
+        <v>8.8787929000000002E-2</v>
+      </c>
+      <c r="G53">
+        <v>2.7722139999999998E-3</v>
+      </c>
+      <c r="H53">
+        <v>0.99639685600000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54">
+        <v>6.1575900000000001E-4</v>
+      </c>
+      <c r="C54">
+        <v>1999.9767119999999</v>
+      </c>
+      <c r="D54">
+        <v>0.40001579300000001</v>
+      </c>
+      <c r="E54">
+        <v>2.3810701E-2</v>
+      </c>
+      <c r="F54">
+        <v>9.3052383000000002E-2</v>
+      </c>
+      <c r="G54">
+        <v>1.4778720000000001E-3</v>
+      </c>
+      <c r="H54">
+        <v>0.99505876199999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>5.7284199999999995E-4</v>
+      </c>
+      <c r="C55">
+        <v>2000.4061589999999</v>
+      </c>
+      <c r="D55">
+        <v>0.40002267499999999</v>
+      </c>
+      <c r="E55">
+        <v>2.5438157999999999E-2</v>
+      </c>
+      <c r="F55">
+        <v>8.9342075000000007E-2</v>
+      </c>
+      <c r="G55">
+        <v>1.5362749999999999E-3</v>
+      </c>
+      <c r="H55">
+        <v>0.99545406299999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56">
+        <v>7.3430900000000005E-4</v>
+      </c>
+      <c r="C56">
+        <v>2000.6603399999999</v>
+      </c>
+      <c r="D56">
+        <v>0.50012684799999996</v>
+      </c>
+      <c r="E56">
+        <v>2.6662858000000001E-2</v>
+      </c>
+      <c r="F56">
+        <v>8.9674559000000001E-2</v>
+      </c>
+      <c r="G56">
+        <v>3.0504239999999999E-3</v>
+      </c>
+      <c r="H56">
+        <v>0.99543250999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="C57">
+        <v>160</v>
+      </c>
+      <c r="D57">
+        <v>0.2</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>9.6295699999999996E-4</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>2.81E-4</v>
+      </c>
+      <c r="C58">
+        <v>160</v>
+      </c>
+      <c r="D58">
+        <v>0.2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>5.4068499999999995E-4</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>3.0699999999999998E-4</v>
+      </c>
+      <c r="C59">
+        <v>160</v>
+      </c>
+      <c r="D59">
+        <v>0.2</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>5.7356200000000001E-4</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="C60">
+        <v>160</v>
+      </c>
+      <c r="D60">
+        <v>0.2</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>1.609114E-3</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>4.3100000000000001E-4</v>
+      </c>
+      <c r="C61">
+        <v>160</v>
+      </c>
+      <c r="D61">
+        <v>0.2</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>2.0221039999999998E-3</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>5.3200000000000003E-4</v>
+      </c>
+      <c r="C62">
+        <v>160</v>
+      </c>
+      <c r="D62">
+        <v>0.2</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>1.858317E-3</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>6.8900000000000005E-4</v>
+      </c>
+      <c r="C63">
+        <v>160</v>
+      </c>
+      <c r="D63">
+        <v>0.2</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>1.541461E-3</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>1.281E-3</v>
+      </c>
+      <c r="C64">
+        <v>160</v>
+      </c>
+      <c r="D64">
+        <v>0.2</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>1.2030529999999999E-3</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>2.52E-4</v>
+      </c>
+      <c r="C65">
+        <v>200</v>
+      </c>
+      <c r="D65">
+        <v>0.2</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>2.27729E-4</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C66">
+        <v>200</v>
+      </c>
+      <c r="D66">
+        <v>0.2</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>1.347741E-3</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>3.2499999999999999E-4</v>
+      </c>
+      <c r="C67">
+        <v>200</v>
+      </c>
+      <c r="D67">
+        <v>0.2</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>1.48168E-3</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>3.8299999999999999E-4</v>
+      </c>
+      <c r="C68">
+        <v>200</v>
+      </c>
+      <c r="D68">
+        <v>0.2</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>1.5823530000000001E-3</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>4.64E-4</v>
+      </c>
+      <c r="C69">
+        <v>200</v>
+      </c>
+      <c r="D69">
+        <v>0.2</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1.264077E-3</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>5.8399999999999999E-4</v>
+      </c>
+      <c r="C70">
+        <v>200</v>
+      </c>
+      <c r="D70">
+        <v>0.2</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>1.7501089999999999E-3</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>7.8799999999999996E-4</v>
+      </c>
+      <c r="C71">
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <v>0.2</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1.2385709999999999E-3</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>1.0950000000000001E-3</v>
+      </c>
+      <c r="C72">
+        <v>200</v>
+      </c>
+      <c r="D72">
+        <v>0.2</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>9.1166800000000003E-4</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C73">
+        <v>200</v>
+      </c>
+      <c r="D73">
+        <v>0.2</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>4.5693399999999999E-4</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>2.7099999999999997E-4</v>
+      </c>
+      <c r="C74">
+        <v>240</v>
+      </c>
+      <c r="D74">
+        <v>0.2</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>5.6943599999999999E-4</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>2.9799999999999998E-4</v>
+      </c>
+      <c r="C75">
+        <v>240</v>
+      </c>
+      <c r="D75">
+        <v>0.2</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1.764112E-3</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>3.4299999999999999E-4</v>
+      </c>
+      <c r="C76">
+        <v>240</v>
+      </c>
+      <c r="D76">
+        <v>0.2</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>2.7815829999999998E-3</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>4.0400000000000001E-4</v>
+      </c>
+      <c r="C77">
+        <v>240</v>
+      </c>
+      <c r="D77">
+        <v>0.2</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>3.124384E-3</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>5.0299999999999997E-4</v>
+      </c>
+      <c r="C78">
+        <v>240</v>
+      </c>
+      <c r="D78">
+        <v>0.2</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>3.5047860000000002E-3</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>6.0999999999999997E-4</v>
+      </c>
+      <c r="C79">
+        <v>240</v>
+      </c>
+      <c r="D79">
+        <v>0.2</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>3.015471E-3</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>8.0400000000000003E-4</v>
+      </c>
+      <c r="C80">
+        <v>240</v>
+      </c>
+      <c r="D80">
+        <v>0.2</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>2.3056370000000001E-3</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>1.0920000000000001E-3</v>
+      </c>
+      <c r="C81">
+        <v>240</v>
+      </c>
+      <c r="D81">
+        <v>0.2</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>1.8617429999999999E-3</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>1.4159999999999999E-3</v>
+      </c>
+      <c r="C82">
+        <v>240</v>
+      </c>
+      <c r="D82">
+        <v>0.2</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>9.7170399999999999E-4</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>2.5399999999999999E-4</v>
+      </c>
+      <c r="C83">
+        <v>280</v>
+      </c>
+      <c r="D83">
+        <v>0.2</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>6.6906099999999998E-4</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>2.9399999999999999E-4</v>
+      </c>
+      <c r="C84">
+        <v>280</v>
+      </c>
+      <c r="D84">
+        <v>0.2</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>2.4819130000000001E-3</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <v>3.3700000000000001E-4</v>
+      </c>
+      <c r="C85">
+        <v>280</v>
+      </c>
+      <c r="D85">
+        <v>0.2</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>3.5047860000000002E-3</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>4.0200000000000001E-4</v>
+      </c>
+      <c r="C86">
+        <v>280</v>
+      </c>
+      <c r="D86">
+        <v>0.2</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>3.5300269999999998E-3</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>4.9700000000000005E-4</v>
+      </c>
+      <c r="C87">
+        <v>280</v>
+      </c>
+      <c r="D87">
+        <v>0.2</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>3.7511160000000001E-3</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>6.1700000000000004E-4</v>
+      </c>
+      <c r="C88">
+        <v>280</v>
+      </c>
+      <c r="D88">
+        <v>0.2</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>3.7918209999999999E-3</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C89">
+        <v>280</v>
+      </c>
+      <c r="D89">
+        <v>0.2</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>2.9280959999999998E-3</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <v>1.0989999999999999E-3</v>
+      </c>
+      <c r="C90">
+        <v>280</v>
+      </c>
+      <c r="D90">
+        <v>0.2</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>2.4002030000000001E-3</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>1.2780000000000001E-3</v>
+      </c>
+      <c r="C91">
+        <v>280</v>
+      </c>
+      <c r="D91">
+        <v>0.2</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>1.534342E-3</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="C92">
+        <v>2050</v>
+      </c>
+      <c r="D92">
+        <v>0.3</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>9.0499999999999999E-4</v>
+      </c>
+      <c r="C93">
+        <v>2350</v>
+      </c>
+      <c r="D93">
+        <v>0.5</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>6.3250000000000003E-4</v>
+      </c>
+      <c r="C94">
+        <v>1600</v>
+      </c>
+      <c r="D94">
+        <v>0.3</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95">
+        <v>6.0749999999999997E-4</v>
+      </c>
+      <c r="C95">
+        <v>1500</v>
+      </c>
+      <c r="D95">
+        <v>0.3</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96">
+        <v>7.3800000000000005E-4</v>
+      </c>
+      <c r="C96">
+        <v>1450</v>
+      </c>
+      <c r="D96">
+        <v>0.5</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97">
+        <v>8.6499999999999999E-4</v>
+      </c>
+      <c r="C97">
+        <v>1850</v>
+      </c>
+      <c r="D97">
+        <v>0.5</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>6.2750000000000002E-4</v>
+      </c>
+      <c r="C98">
+        <v>1600</v>
+      </c>
+      <c r="D98">
+        <v>0.3</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99">
+        <v>5.8500000000000002E-4</v>
+      </c>
+      <c r="C99">
+        <v>1450</v>
+      </c>
+      <c r="D99">
+        <v>0.3</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100">
+        <v>7.0750000000000001E-4</v>
+      </c>
+      <c r="C100">
+        <v>1400</v>
+      </c>
+      <c r="D100">
+        <v>0.5</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101">
+        <v>6.3500000000000004E-4</v>
+      </c>
+      <c r="C101">
+        <v>1150</v>
+      </c>
+      <c r="D101">
+        <v>0.5</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <v>6.6750000000000002E-4</v>
+      </c>
+      <c r="C102">
+        <v>1600</v>
+      </c>
+      <c r="D102">
+        <v>0.3</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>6.3029999999999998E-4</v>
+      </c>
+      <c r="C103">
+        <v>1500</v>
+      </c>
+      <c r="D103">
+        <v>0.3</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104">
+        <v>7.2250000000000005E-4</v>
+      </c>
+      <c r="C104">
+        <v>1350</v>
+      </c>
+      <c r="D104">
+        <v>0.5</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105">
+        <v>6.7250000000000003E-4</v>
+      </c>
+      <c r="C105">
+        <v>1200</v>
+      </c>
+      <c r="D105">
+        <v>0.5</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added column h_dis_0 for data_main.xlsx > detail_V_dis.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagr9\Projekte\MA\MA-Model_3\Separator Model\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Projekte\MA-Model_3\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4B3506-46E1-4AF3-A88C-9FD61A206621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680AAE82-45C1-450F-B1FF-3DB9E270E7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="22">
   <si>
     <t>exp</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>h_c_0</t>
+  </si>
+  <si>
+    <t>h_dis_0</t>
   </si>
 </sst>
 </file>
@@ -11883,8 +11886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20356976-3232-4BA6-902F-5E9FBCFC61E6}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11903,7 +11906,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>20</v>
@@ -11929,7 +11932,7 @@
         <v>0.29701893400000001</v>
       </c>
       <c r="E2">
-        <v>3.6502927999999997E-2</v>
+        <v>3.55819E-2</v>
       </c>
       <c r="F2">
         <v>9.6633421999999997E-2</v>
@@ -11955,7 +11958,7 @@
         <v>0.50333939500000002</v>
       </c>
       <c r="E3">
-        <v>2.8484735000000001E-2</v>
+        <v>2.2846333E-2</v>
       </c>
       <c r="F3">
         <v>9.2660582000000005E-2</v>
@@ -11981,7 +11984,7 @@
         <v>0.49988101000000001</v>
       </c>
       <c r="E4">
-        <v>3.8919571E-2</v>
+        <v>3.3656999999999999E-2</v>
       </c>
       <c r="F4">
         <v>0.10772396300000001</v>
@@ -12007,7 +12010,7 @@
         <v>0.399764919</v>
       </c>
       <c r="E5">
-        <v>3.8463404E-2</v>
+        <v>3.2073999999999998E-2</v>
       </c>
       <c r="F5">
         <v>9.5001253999999993E-2</v>
@@ -12033,7 +12036,7 @@
         <v>0.50015754999999995</v>
       </c>
       <c r="E6">
-        <v>4.0361706999999997E-2</v>
+        <v>3.8374125000000002E-2</v>
       </c>
       <c r="F6">
         <v>0.101830843</v>
@@ -12059,7 +12062,7 @@
         <v>0.49989457599999998</v>
       </c>
       <c r="E7">
-        <v>3.8023349999999997E-2</v>
+        <v>3.2000428999999997E-2</v>
       </c>
       <c r="F7">
         <v>0.108397884</v>
@@ -12085,7 +12088,7 @@
         <v>0.40002338700000001</v>
       </c>
       <c r="E8">
-        <v>6.6916982E-2</v>
+        <v>2.9817666999999999E-2</v>
       </c>
       <c r="F8">
         <v>0.106790285</v>
@@ -12111,7 +12114,7 @@
         <v>0.29988877800000002</v>
       </c>
       <c r="E9">
-        <v>3.6448479999999998E-2</v>
+        <v>2.9670385000000001E-2</v>
       </c>
       <c r="F9">
         <v>0.10019613600000001</v>
@@ -12137,7 +12140,7 @@
         <v>0.50033280999999996</v>
       </c>
       <c r="E10">
-        <v>3.7521118999999999E-2</v>
+        <v>2.9766384999999999E-2</v>
       </c>
       <c r="F10">
         <v>9.8495864000000002E-2</v>
@@ -12163,7 +12166,7 @@
         <v>0.30092750000000001</v>
       </c>
       <c r="E11">
-        <v>3.3229887E-2</v>
+        <v>3.4920187999999998E-2</v>
       </c>
       <c r="F11">
         <v>0.100884113</v>
@@ -12189,7 +12192,7 @@
         <v>0.40003253100000002</v>
       </c>
       <c r="E12">
-        <v>7.0955006000000001E-2</v>
+        <v>1.9631529000000002E-2</v>
       </c>
       <c r="F12">
         <v>0.11041532699999999</v>
@@ -12215,7 +12218,7 @@
         <v>0.49949943499999999</v>
       </c>
       <c r="E13">
-        <v>4.2382797999999999E-2</v>
+        <v>4.1055332999999999E-2</v>
       </c>
       <c r="F13">
         <v>9.7580385000000006E-2</v>
@@ -12241,7 +12244,7 @@
         <v>0.27718706700000001</v>
       </c>
       <c r="E14">
-        <v>3.6368708E-2</v>
+        <v>1.9585846000000001E-2</v>
       </c>
       <c r="F14">
         <v>0.103970942</v>
@@ -12267,7 +12270,7 @@
         <v>0.499859416</v>
       </c>
       <c r="E15">
-        <v>1.8851822000000001E-2</v>
+        <v>1.5360333E-2</v>
       </c>
       <c r="F15">
         <v>0.10280117799999999</v>
@@ -12293,7 +12296,7 @@
         <v>0.29920427599999999</v>
       </c>
       <c r="E16">
-        <v>4.1816536000000001E-2</v>
+        <v>3.5955842000000002E-2</v>
       </c>
       <c r="F16">
         <v>0.101860464</v>
@@ -12319,7 +12322,7 @@
         <v>0.40006547100000001</v>
       </c>
       <c r="E17">
-        <v>2.4784075999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>9.7689174000000004E-2</v>
@@ -12345,7 +12348,7 @@
         <v>0.49991358299999999</v>
       </c>
       <c r="E18">
-        <v>1.8550810000000001E-2</v>
+        <v>1.5761217000000001E-2</v>
       </c>
       <c r="F18">
         <v>9.4884389999999999E-2</v>
@@ -12371,7 +12374,7 @@
         <v>0.30006925000000001</v>
       </c>
       <c r="E19">
-        <v>3.6809690999999999E-2</v>
+        <v>2.6276999999999998E-2</v>
       </c>
       <c r="F19">
         <v>0.108183192</v>
@@ -12397,7 +12400,7 @@
         <v>0.29996158899999997</v>
       </c>
       <c r="E20">
-        <v>1.9367124999999999E-2</v>
+        <v>1.6771635999999999E-2</v>
       </c>
       <c r="F20">
         <v>9.7314092000000005E-2</v>
@@ -12423,7 +12426,7 @@
         <v>0.49965211700000001</v>
       </c>
       <c r="E21">
-        <v>4.2670694000000002E-2</v>
+        <v>3.9373499999999999E-2</v>
       </c>
       <c r="F21">
         <v>0.10375522299999999</v>
@@ -12449,7 +12452,7 @@
         <v>0.50001522700000001</v>
       </c>
       <c r="E22">
-        <v>1.9893559000000002E-2</v>
+        <v>1.5923438000000002E-2</v>
       </c>
       <c r="F22">
         <v>9.5239508E-2</v>
@@ -12475,7 +12478,7 @@
         <v>0.30000356700000003</v>
       </c>
       <c r="E23">
-        <v>5.1118615999999999E-2</v>
+        <v>2.9010142999999999E-2</v>
       </c>
       <c r="F23">
         <v>0.114449734</v>
@@ -12501,7 +12504,7 @@
         <v>0.50013415000000006</v>
       </c>
       <c r="E24">
-        <v>5.7089112999999997E-2</v>
+        <v>2.9240461999999998E-2</v>
       </c>
       <c r="F24">
         <v>0.11521322000000001</v>
@@ -12527,7 +12530,7 @@
         <v>0.40118413600000002</v>
       </c>
       <c r="E25">
-        <v>4.5435773999999998E-2</v>
+        <v>3.6132938000000003E-2</v>
       </c>
       <c r="F25">
         <v>0.10055367599999999</v>
@@ -12553,7 +12556,7 @@
         <v>0.30087852900000001</v>
       </c>
       <c r="E26">
-        <v>7.5760642000000003E-2</v>
+        <v>2.4022870000000002E-2</v>
       </c>
       <c r="F26">
         <v>0.10911349100000001</v>
@@ -12579,7 +12582,7 @@
         <v>0.29883443599999998</v>
       </c>
       <c r="E27">
-        <v>6.6170259999999995E-2</v>
+        <v>2.9332111000000001E-2</v>
       </c>
       <c r="F27">
         <v>0.11349644</v>
@@ -12605,7 +12608,7 @@
         <v>0.50009379399999998</v>
       </c>
       <c r="E28">
-        <v>5.5513298000000003E-2</v>
+        <v>3.3174416999999998E-2</v>
       </c>
       <c r="F28">
         <v>0.114298685</v>
@@ -12631,7 +12634,7 @@
         <v>0.29980042600000001</v>
       </c>
       <c r="E29">
-        <v>3.1885854999999998E-2</v>
+        <v>2.8255058999999999E-2</v>
       </c>
       <c r="F29">
         <v>0.10856081200000001</v>
@@ -12657,7 +12660,7 @@
         <v>0.29999618500000003</v>
       </c>
       <c r="E30">
-        <v>4.7035642000000003E-2</v>
+        <v>4.2983100000000003E-2</v>
       </c>
       <c r="F30">
         <v>0.10975439100000001</v>
@@ -12683,7 +12686,7 @@
         <v>0.300016848</v>
       </c>
       <c r="E31">
-        <v>4.267257E-2</v>
+        <v>3.03678E-2</v>
       </c>
       <c r="F31">
         <v>0.107568497</v>
@@ -12709,7 +12712,7 @@
         <v>0.29999587</v>
       </c>
       <c r="E32">
-        <v>4.6113999000000003E-2</v>
+        <v>2.3775000000000001E-2</v>
       </c>
       <c r="F32">
         <v>0.11548971800000001</v>
@@ -12735,7 +12738,7 @@
         <v>0.30007985999999998</v>
       </c>
       <c r="E33">
-        <v>3.1432143000000003E-2</v>
+        <v>2.7580614999999999E-2</v>
       </c>
       <c r="F33">
         <v>0.11381099</v>
@@ -12761,7 +12764,7 @@
         <v>0.30001281800000001</v>
       </c>
       <c r="E34">
-        <v>3.3010744000000002E-2</v>
+        <v>2.8364166999999999E-2</v>
       </c>
       <c r="F34">
         <v>0.11308117199999999</v>
@@ -12787,7 +12790,7 @@
         <v>0.39999618199999998</v>
       </c>
       <c r="E35">
-        <v>6.9506928999999995E-2</v>
+        <v>3.9580443999999999E-2</v>
       </c>
       <c r="F35">
         <v>0.110695898</v>
@@ -12813,7 +12816,7 @@
         <v>0.49995556099999999</v>
       </c>
       <c r="E36">
-        <v>4.8558603999999998E-2</v>
+        <v>4.6688437999999999E-2</v>
       </c>
       <c r="F36">
         <v>9.5985962999999994E-2</v>
@@ -12839,7 +12842,7 @@
         <v>0.39989443400000002</v>
       </c>
       <c r="E37">
-        <v>4.1705930000000002E-2</v>
+        <v>3.2895832999999999E-2</v>
       </c>
       <c r="F37">
         <v>0.10475915299999999</v>
@@ -12865,7 +12868,7 @@
         <v>0.49920661399999999</v>
       </c>
       <c r="E38">
-        <v>4.8344787E-2</v>
+        <v>2.7389750000000001E-2</v>
       </c>
       <c r="F38">
         <v>0.12562072899999999</v>
@@ -12891,7 +12894,7 @@
         <v>0.40056073800000003</v>
       </c>
       <c r="E39">
-        <v>7.1139833E-2</v>
+        <v>3.3499599999999997E-2</v>
       </c>
       <c r="F39">
         <v>0.11312243299999999</v>
@@ -12917,7 +12920,7 @@
         <v>0.49692148400000002</v>
       </c>
       <c r="E40">
-        <v>2.3973168999999999E-2</v>
+        <v>1.6203833000000001E-2</v>
       </c>
       <c r="F40">
         <v>9.1711663999999998E-2</v>
@@ -12943,7 +12946,7 @@
         <v>0.50025813699999999</v>
       </c>
       <c r="E41">
-        <v>2.6577284999999999E-2</v>
+        <v>2.5555333E-2</v>
       </c>
       <c r="F41">
         <v>9.2475197999999995E-2</v>
@@ -12969,7 +12972,7 @@
         <v>0.50000099099999995</v>
       </c>
       <c r="E42">
-        <v>2.6915963000000001E-2</v>
+        <v>2.7710216999999999E-2</v>
       </c>
       <c r="F42">
         <v>9.1934420000000003E-2</v>
@@ -12995,7 +12998,7 @@
         <v>0.49990232400000001</v>
       </c>
       <c r="E43">
-        <v>2.4668497000000001E-2</v>
+        <v>1.9429286E-2</v>
       </c>
       <c r="F43">
         <v>9.1588153000000005E-2</v>
@@ -13021,7 +13024,7 @@
         <v>0.29994249899999997</v>
       </c>
       <c r="E44">
-        <v>2.6047677000000002E-2</v>
+        <v>2.6298999999999999E-2</v>
       </c>
       <c r="F44">
         <v>0.10857765</v>
@@ -13047,7 +13050,7 @@
         <v>0.30007125099999998</v>
       </c>
       <c r="E45">
-        <v>1.9110674000000001E-2</v>
+        <v>1.9176444000000001E-2</v>
       </c>
       <c r="F45">
         <v>0.12915310899999999</v>
@@ -13073,7 +13076,7 @@
         <v>0.39993976599999997</v>
       </c>
       <c r="E46">
-        <v>2.7369943000000001E-2</v>
+        <v>4.5705333000000001E-2</v>
       </c>
       <c r="F46">
         <v>9.7766817000000006E-2</v>
@@ -13099,7 +13102,7 @@
         <v>0.50044513199999996</v>
       </c>
       <c r="E47">
-        <v>2.0620128000000001E-2</v>
+        <v>2.2795666999999999E-2</v>
       </c>
       <c r="F47">
         <v>0.103834646</v>
@@ -13125,7 +13128,7 @@
         <v>0.499986655</v>
       </c>
       <c r="E48">
-        <v>2.1720821000000001E-2</v>
+        <v>2.3137000000000001E-2</v>
       </c>
       <c r="F48">
         <v>0.103615651</v>
@@ -13151,7 +13154,7 @@
         <v>0.40017336999999997</v>
       </c>
       <c r="E49">
-        <v>2.0735538000000001E-2</v>
+        <v>1.6598000000000002E-2</v>
       </c>
       <c r="F49">
         <v>9.4777095000000006E-2</v>
@@ -13177,7 +13180,7 @@
         <v>0.40074769799999999</v>
       </c>
       <c r="E50">
-        <v>2.2464746000000001E-2</v>
+        <v>1.9850666999999999E-2</v>
       </c>
       <c r="F50">
         <v>9.4852504000000004E-2</v>
@@ -13203,7 +13206,7 @@
         <v>0.50002069100000002</v>
       </c>
       <c r="E51">
-        <v>2.4334100000000001E-2</v>
+        <v>2.4327778000000001E-2</v>
       </c>
       <c r="F51">
         <v>9.0262732999999998E-2</v>
@@ -13229,7 +13232,7 @@
         <v>0.49970003499999999</v>
       </c>
       <c r="E52">
-        <v>2.3888031000000001E-2</v>
+        <v>2.9573833000000001E-2</v>
       </c>
       <c r="F52">
         <v>0.101849986</v>
@@ -13255,7 +13258,7 @@
         <v>0.49998881699999997</v>
       </c>
       <c r="E53">
-        <v>2.6883537999999998E-2</v>
+        <v>2.3282932999999999E-2</v>
       </c>
       <c r="F53">
         <v>8.8787929000000002E-2</v>
@@ -13281,7 +13284,7 @@
         <v>0.40001579300000001</v>
       </c>
       <c r="E54">
-        <v>2.3810701E-2</v>
+        <v>3.4569500000000003E-2</v>
       </c>
       <c r="F54">
         <v>9.3052383000000002E-2</v>
@@ -13307,7 +13310,7 @@
         <v>0.40002267499999999</v>
       </c>
       <c r="E55">
-        <v>2.5438157999999999E-2</v>
+        <v>2.1106E-2</v>
       </c>
       <c r="F55">
         <v>8.9342075000000007E-2</v>
@@ -13333,7 +13336,7 @@
         <v>0.50012684799999996</v>
       </c>
       <c r="E56">
-        <v>2.6662858000000001E-2</v>
+        <v>2.0743889000000001E-2</v>
       </c>
       <c r="F56">
         <v>8.9674559000000001E-2</v>

</xml_diff>